<commit_message>
Corrected tests to precreate containers into the container handler hash to avoid attempts to access via solr.
</commit_message>
<xml_diff>
--- a/backend/spec/fixtures/bulk_import/testTopLinkerUpload.xlsx
+++ b/backend/spec/fixtures/bulk_import/testTopLinkerUpload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vac765/git/archivesspace-bulk/backend/spec/fixtures/bulk_import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vac765/git/harvard-archivesspace/backend/spec/fixtures/bulk_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E19734D-A28C-E543-9374-E53368EA80D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBE5B2E-27D7-0544-A4BB-B011AE9614F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="23920" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7:P10"/>
+      <selection activeCell="M7" sqref="M7:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1214,7 +1214,7 @@
         <v>56</v>
       </c>
       <c r="M6">
-        <v>54555</v>
+        <v>54556</v>
       </c>
       <c r="N6">
         <v>43587</v>
@@ -1267,7 +1267,7 @@
         <v>56</v>
       </c>
       <c r="M7">
-        <v>54555</v>
+        <v>54556</v>
       </c>
       <c r="N7">
         <v>43587</v>
@@ -1320,7 +1320,7 @@
         <v>56</v>
       </c>
       <c r="M8">
-        <v>54555</v>
+        <v>54556</v>
       </c>
       <c r="N8">
         <v>43587</v>
@@ -1355,7 +1355,7 @@
         <v>49</v>
       </c>
       <c r="J9">
-        <v>154691</v>
+        <v>4</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>55</v>
@@ -1375,7 +1375,7 @@
         <v>49</v>
       </c>
       <c r="J10">
-        <v>154692</v>
+        <v>4</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>55</v>

</xml_diff>